<commit_message>
trial 06 st complete
</commit_message>
<xml_diff>
--- a/asc_data/processed/set_03/WDS_3_3_4_11_ASCOF_1A.xlsx
+++ b/asc_data/processed/set_03/WDS_3_3_4_11_ASCOF_1A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trubens/verde_repos/verde/asc_data/processed/set_03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16D6150-D9E1-074A-9F9E-5DDF0E1D8F66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A515D0F-84B2-DE4B-A024-4922118EC1A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="-19400" windowWidth="32480" windowHeight="15440" xr2:uid="{90971CAB-A660-204C-849C-7B4EE75AA156}"/>
+    <workbookView xWindow="1020" yWindow="5440" windowWidth="32480" windowHeight="15440" activeTab="3" xr2:uid="{90971CAB-A660-204C-849C-7B4EE75AA156}"/>
   </bookViews>
   <sheets>
     <sheet name="wide" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="tidy_gender_qol" sheetId="6" r:id="rId3"/>
     <sheet name="tidy_age_qol" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -197,7 +197,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -238,7 +238,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6232059F-6528-7544-8563-E7A2B92C749E}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1161,7 +1161,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD54"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1879,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9301273-4308-CE4E-B42B-4CE1AF94E258}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD30"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2193,8 +2193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C29DBD-3BC7-074F-AA17-A3CCB01AEAC4}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD26"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>